<commit_message>
Libs hinzugefügt Interface für Hibernate Angelegt Lere GiveMeAMessage class
</commit_message>
<xml_diff>
--- a/GiveMeTheREST-API-Definition.xlsx
+++ b/GiveMeTheREST-API-Definition.xlsx
@@ -32,9 +32,6 @@
     <t>Address:</t>
   </si>
   <si>
-    <t>http://schattenhauer.de/GiveMeTheRESTServer/ FUNCTION</t>
-  </si>
-  <si>
     <t>FUNCTION</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>msg/root</t>
+  </si>
+  <si>
+    <t>http://schattenhauer.de/GiveMeTheRESTServer/rest/ FUNCTION</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,123 +497,123 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1"/>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
       <c r="G9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2"/>
       <c r="G10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2"/>
       <c r="G11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>